<commit_message>
Update journal and doc
</commit_message>
<xml_diff>
--- a/doc/Pianificazione.xlsx
+++ b/doc/Pianificazione.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="28">
   <si>
     <t>ATTIVITÀ</t>
   </si>
@@ -782,21 +782,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -817,6 +802,36 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -841,21 +856,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,11 +1183,11 @@
   </sheetPr>
   <dimension ref="A1:DS35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="BT27" sqref="BT27"/>
+      <selection pane="bottomRight" activeCell="CQ32" sqref="CQ32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1195,7 +1195,9 @@
     <col min="1" max="1" width="3.7109375" style="32" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" style="32" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="32" customWidth="1"/>
-    <col min="4" max="135" width="1.85546875" style="32" customWidth="1"/>
+    <col min="4" max="73" width="1.85546875" style="32" customWidth="1"/>
+    <col min="74" max="93" width="1.85546875" style="32" hidden="1" customWidth="1"/>
+    <col min="94" max="135" width="1.85546875" style="32" customWidth="1"/>
     <col min="136" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
@@ -1238,23 +1240,23 @@
       <c r="AI2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AN2" s="111">
+      <c r="AN2" s="104">
         <v>43202</v>
       </c>
-      <c r="AO2" s="111"/>
-      <c r="AP2" s="111"/>
-      <c r="AQ2" s="111"/>
-      <c r="AR2" s="111"/>
-      <c r="AS2" s="111"/>
-      <c r="AT2" s="111"/>
-      <c r="AV2" s="110"/>
-      <c r="AW2" s="110"/>
-      <c r="AX2" s="110"/>
-      <c r="AY2" s="110"/>
-      <c r="AZ2" s="110"/>
-      <c r="BA2" s="110"/>
-      <c r="BB2" s="110"/>
-      <c r="BC2" s="110"/>
+      <c r="AO2" s="104"/>
+      <c r="AP2" s="104"/>
+      <c r="AQ2" s="104"/>
+      <c r="AR2" s="104"/>
+      <c r="AS2" s="104"/>
+      <c r="AT2" s="104"/>
+      <c r="AV2" s="103"/>
+      <c r="AW2" s="103"/>
+      <c r="AX2" s="103"/>
+      <c r="AY2" s="103"/>
+      <c r="AZ2" s="103"/>
+      <c r="BA2" s="103"/>
+      <c r="BB2" s="103"/>
+      <c r="BC2" s="103"/>
     </row>
     <row r="3" spans="1:123" s="1" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
@@ -1354,501 +1356,501 @@
       <c r="AI4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AN4" s="112">
+      <c r="AN4" s="105">
         <v>43235</v>
       </c>
-      <c r="AO4" s="113"/>
-      <c r="AP4" s="113"/>
-      <c r="AQ4" s="113"/>
-      <c r="AR4" s="113"/>
-      <c r="AS4" s="113"/>
-      <c r="AT4" s="113"/>
-      <c r="AV4" s="110"/>
-      <c r="AW4" s="110"/>
-      <c r="AX4" s="110"/>
-      <c r="AY4" s="110"/>
-      <c r="AZ4" s="110"/>
-      <c r="BA4" s="110"/>
-      <c r="BB4" s="110"/>
-      <c r="BC4" s="110"/>
-      <c r="BH4" s="114"/>
-      <c r="BI4" s="114"/>
+      <c r="AO4" s="106"/>
+      <c r="AP4" s="106"/>
+      <c r="AQ4" s="106"/>
+      <c r="AR4" s="106"/>
+      <c r="AS4" s="106"/>
+      <c r="AT4" s="106"/>
+      <c r="AV4" s="103"/>
+      <c r="AW4" s="103"/>
+      <c r="AX4" s="103"/>
+      <c r="AY4" s="103"/>
+      <c r="AZ4" s="103"/>
+      <c r="BA4" s="103"/>
+      <c r="BB4" s="103"/>
+      <c r="BC4" s="103"/>
+      <c r="BH4" s="102"/>
+      <c r="BI4" s="102"/>
     </row>
     <row r="5" spans="1:123" s="1" customFormat="1" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:123" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="105"/>
-      <c r="B6" s="106"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="95">
+      <c r="D6" s="90">
         <v>43202</v>
       </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="97"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="97"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="95">
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="90">
         <v>43203</v>
       </c>
-      <c r="O6" s="96"/>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="96"/>
-      <c r="R6" s="97"/>
-      <c r="S6" s="97"/>
-      <c r="T6" s="97"/>
-      <c r="U6" s="97"/>
-      <c r="V6" s="97"/>
-      <c r="W6" s="98"/>
-      <c r="X6" s="95">
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="92"/>
+      <c r="S6" s="92"/>
+      <c r="T6" s="92"/>
+      <c r="U6" s="92"/>
+      <c r="V6" s="92"/>
+      <c r="W6" s="93"/>
+      <c r="X6" s="90">
         <v>43206</v>
       </c>
-      <c r="Y6" s="96"/>
-      <c r="Z6" s="96"/>
-      <c r="AA6" s="96"/>
-      <c r="AB6" s="97"/>
-      <c r="AC6" s="97"/>
-      <c r="AD6" s="97"/>
-      <c r="AE6" s="97"/>
-      <c r="AF6" s="97"/>
-      <c r="AG6" s="98"/>
-      <c r="AH6" s="95">
+      <c r="Y6" s="91"/>
+      <c r="Z6" s="91"/>
+      <c r="AA6" s="91"/>
+      <c r="AB6" s="92"/>
+      <c r="AC6" s="92"/>
+      <c r="AD6" s="92"/>
+      <c r="AE6" s="92"/>
+      <c r="AF6" s="92"/>
+      <c r="AG6" s="93"/>
+      <c r="AH6" s="90">
         <v>43207</v>
       </c>
-      <c r="AI6" s="96"/>
-      <c r="AJ6" s="96"/>
-      <c r="AK6" s="96"/>
-      <c r="AL6" s="97"/>
-      <c r="AM6" s="97"/>
-      <c r="AN6" s="97"/>
-      <c r="AO6" s="97"/>
-      <c r="AP6" s="97"/>
-      <c r="AQ6" s="98"/>
-      <c r="AR6" s="95">
+      <c r="AI6" s="91"/>
+      <c r="AJ6" s="91"/>
+      <c r="AK6" s="91"/>
+      <c r="AL6" s="92"/>
+      <c r="AM6" s="92"/>
+      <c r="AN6" s="92"/>
+      <c r="AO6" s="92"/>
+      <c r="AP6" s="92"/>
+      <c r="AQ6" s="93"/>
+      <c r="AR6" s="90">
         <v>43216</v>
       </c>
-      <c r="AS6" s="96"/>
-      <c r="AT6" s="96"/>
-      <c r="AU6" s="96"/>
-      <c r="AV6" s="97"/>
-      <c r="AW6" s="97"/>
-      <c r="AX6" s="97"/>
-      <c r="AY6" s="97"/>
-      <c r="AZ6" s="97"/>
-      <c r="BA6" s="98"/>
-      <c r="BB6" s="95">
+      <c r="AS6" s="91"/>
+      <c r="AT6" s="91"/>
+      <c r="AU6" s="91"/>
+      <c r="AV6" s="92"/>
+      <c r="AW6" s="92"/>
+      <c r="AX6" s="92"/>
+      <c r="AY6" s="92"/>
+      <c r="AZ6" s="92"/>
+      <c r="BA6" s="93"/>
+      <c r="BB6" s="90">
         <v>43217</v>
       </c>
-      <c r="BC6" s="96"/>
-      <c r="BD6" s="96"/>
-      <c r="BE6" s="96"/>
-      <c r="BF6" s="97"/>
-      <c r="BG6" s="97"/>
-      <c r="BH6" s="97"/>
-      <c r="BI6" s="97"/>
-      <c r="BJ6" s="97"/>
-      <c r="BK6" s="98"/>
-      <c r="BL6" s="95">
+      <c r="BC6" s="91"/>
+      <c r="BD6" s="91"/>
+      <c r="BE6" s="91"/>
+      <c r="BF6" s="92"/>
+      <c r="BG6" s="92"/>
+      <c r="BH6" s="92"/>
+      <c r="BI6" s="92"/>
+      <c r="BJ6" s="92"/>
+      <c r="BK6" s="93"/>
+      <c r="BL6" s="90">
         <v>43220</v>
       </c>
-      <c r="BM6" s="96"/>
-      <c r="BN6" s="96"/>
-      <c r="BO6" s="96"/>
-      <c r="BP6" s="97"/>
-      <c r="BQ6" s="97"/>
-      <c r="BR6" s="97"/>
-      <c r="BS6" s="97"/>
-      <c r="BT6" s="97"/>
-      <c r="BU6" s="98"/>
-      <c r="BV6" s="95">
+      <c r="BM6" s="91"/>
+      <c r="BN6" s="91"/>
+      <c r="BO6" s="91"/>
+      <c r="BP6" s="92"/>
+      <c r="BQ6" s="92"/>
+      <c r="BR6" s="92"/>
+      <c r="BS6" s="92"/>
+      <c r="BT6" s="92"/>
+      <c r="BU6" s="93"/>
+      <c r="BV6" s="90">
         <v>43221</v>
       </c>
-      <c r="BW6" s="96"/>
-      <c r="BX6" s="96"/>
-      <c r="BY6" s="96"/>
-      <c r="BZ6" s="97"/>
-      <c r="CA6" s="97"/>
-      <c r="CB6" s="97"/>
-      <c r="CC6" s="97"/>
-      <c r="CD6" s="97"/>
-      <c r="CE6" s="98"/>
-      <c r="CF6" s="95">
+      <c r="BW6" s="91"/>
+      <c r="BX6" s="91"/>
+      <c r="BY6" s="91"/>
+      <c r="BZ6" s="92"/>
+      <c r="CA6" s="92"/>
+      <c r="CB6" s="92"/>
+      <c r="CC6" s="92"/>
+      <c r="CD6" s="92"/>
+      <c r="CE6" s="93"/>
+      <c r="CF6" s="90">
         <v>43230</v>
       </c>
-      <c r="CG6" s="96"/>
-      <c r="CH6" s="96"/>
-      <c r="CI6" s="96"/>
-      <c r="CJ6" s="97"/>
-      <c r="CK6" s="97"/>
-      <c r="CL6" s="97"/>
-      <c r="CM6" s="97"/>
-      <c r="CN6" s="97"/>
-      <c r="CO6" s="98"/>
-      <c r="CP6" s="95">
+      <c r="CG6" s="91"/>
+      <c r="CH6" s="91"/>
+      <c r="CI6" s="91"/>
+      <c r="CJ6" s="92"/>
+      <c r="CK6" s="92"/>
+      <c r="CL6" s="92"/>
+      <c r="CM6" s="92"/>
+      <c r="CN6" s="92"/>
+      <c r="CO6" s="93"/>
+      <c r="CP6" s="90">
         <v>43231</v>
       </c>
-      <c r="CQ6" s="96"/>
-      <c r="CR6" s="96"/>
-      <c r="CS6" s="96"/>
-      <c r="CT6" s="97"/>
-      <c r="CU6" s="97"/>
-      <c r="CV6" s="97"/>
-      <c r="CW6" s="97"/>
-      <c r="CX6" s="97"/>
-      <c r="CY6" s="98"/>
-      <c r="CZ6" s="95">
+      <c r="CQ6" s="91"/>
+      <c r="CR6" s="91"/>
+      <c r="CS6" s="91"/>
+      <c r="CT6" s="92"/>
+      <c r="CU6" s="92"/>
+      <c r="CV6" s="92"/>
+      <c r="CW6" s="92"/>
+      <c r="CX6" s="92"/>
+      <c r="CY6" s="93"/>
+      <c r="CZ6" s="90">
         <v>43234</v>
       </c>
-      <c r="DA6" s="96"/>
-      <c r="DB6" s="96"/>
-      <c r="DC6" s="96"/>
-      <c r="DD6" s="97"/>
-      <c r="DE6" s="97"/>
-      <c r="DF6" s="97"/>
-      <c r="DG6" s="97"/>
-      <c r="DH6" s="97"/>
-      <c r="DI6" s="98"/>
-      <c r="DJ6" s="95">
+      <c r="DA6" s="91"/>
+      <c r="DB6" s="91"/>
+      <c r="DC6" s="91"/>
+      <c r="DD6" s="92"/>
+      <c r="DE6" s="92"/>
+      <c r="DF6" s="92"/>
+      <c r="DG6" s="92"/>
+      <c r="DH6" s="92"/>
+      <c r="DI6" s="93"/>
+      <c r="DJ6" s="90">
         <v>43235</v>
       </c>
-      <c r="DK6" s="96"/>
-      <c r="DL6" s="96"/>
-      <c r="DM6" s="96"/>
-      <c r="DN6" s="97"/>
-      <c r="DO6" s="97"/>
-      <c r="DP6" s="97"/>
-      <c r="DQ6" s="97"/>
-      <c r="DR6" s="97"/>
-      <c r="DS6" s="98"/>
+      <c r="DK6" s="91"/>
+      <c r="DL6" s="91"/>
+      <c r="DM6" s="91"/>
+      <c r="DN6" s="92"/>
+      <c r="DO6" s="92"/>
+      <c r="DP6" s="92"/>
+      <c r="DQ6" s="92"/>
+      <c r="DR6" s="92"/>
+      <c r="DS6" s="93"/>
     </row>
     <row r="7" spans="1:123" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="107"/>
-      <c r="B7" s="108"/>
+      <c r="A7" s="112"/>
+      <c r="B7" s="113"/>
       <c r="C7" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="99" t="s">
+      <c r="D7" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="101"/>
-      <c r="N7" s="99" t="s">
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100"/>
-      <c r="Q7" s="100"/>
-      <c r="R7" s="100"/>
-      <c r="S7" s="100"/>
-      <c r="T7" s="100"/>
-      <c r="U7" s="100"/>
-      <c r="V7" s="100"/>
-      <c r="W7" s="101"/>
-      <c r="X7" s="99" t="s">
+      <c r="O7" s="95"/>
+      <c r="P7" s="95"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="95"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="95"/>
+      <c r="U7" s="95"/>
+      <c r="V7" s="95"/>
+      <c r="W7" s="96"/>
+      <c r="X7" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="Y7" s="100"/>
-      <c r="Z7" s="100"/>
-      <c r="AA7" s="100"/>
-      <c r="AB7" s="100"/>
-      <c r="AC7" s="100"/>
-      <c r="AD7" s="100"/>
-      <c r="AE7" s="100"/>
-      <c r="AF7" s="100"/>
-      <c r="AG7" s="101"/>
-      <c r="AH7" s="99" t="s">
+      <c r="Y7" s="95"/>
+      <c r="Z7" s="95"/>
+      <c r="AA7" s="95"/>
+      <c r="AB7" s="95"/>
+      <c r="AC7" s="95"/>
+      <c r="AD7" s="95"/>
+      <c r="AE7" s="95"/>
+      <c r="AF7" s="95"/>
+      <c r="AG7" s="96"/>
+      <c r="AH7" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="AI7" s="100"/>
-      <c r="AJ7" s="100"/>
-      <c r="AK7" s="100"/>
-      <c r="AL7" s="100"/>
-      <c r="AM7" s="100"/>
-      <c r="AN7" s="100"/>
-      <c r="AO7" s="100"/>
-      <c r="AP7" s="100"/>
-      <c r="AQ7" s="101"/>
-      <c r="AR7" s="99" t="s">
+      <c r="AI7" s="95"/>
+      <c r="AJ7" s="95"/>
+      <c r="AK7" s="95"/>
+      <c r="AL7" s="95"/>
+      <c r="AM7" s="95"/>
+      <c r="AN7" s="95"/>
+      <c r="AO7" s="95"/>
+      <c r="AP7" s="95"/>
+      <c r="AQ7" s="96"/>
+      <c r="AR7" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="AS7" s="100"/>
-      <c r="AT7" s="100"/>
-      <c r="AU7" s="100"/>
-      <c r="AV7" s="100"/>
-      <c r="AW7" s="100"/>
-      <c r="AX7" s="100"/>
-      <c r="AY7" s="100"/>
-      <c r="AZ7" s="100"/>
-      <c r="BA7" s="101"/>
-      <c r="BB7" s="99" t="s">
+      <c r="AS7" s="95"/>
+      <c r="AT7" s="95"/>
+      <c r="AU7" s="95"/>
+      <c r="AV7" s="95"/>
+      <c r="AW7" s="95"/>
+      <c r="AX7" s="95"/>
+      <c r="AY7" s="95"/>
+      <c r="AZ7" s="95"/>
+      <c r="BA7" s="96"/>
+      <c r="BB7" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="BC7" s="100"/>
-      <c r="BD7" s="100"/>
-      <c r="BE7" s="100"/>
-      <c r="BF7" s="100"/>
-      <c r="BG7" s="100"/>
-      <c r="BH7" s="100"/>
-      <c r="BI7" s="100"/>
-      <c r="BJ7" s="100"/>
-      <c r="BK7" s="101"/>
-      <c r="BL7" s="99" t="s">
+      <c r="BC7" s="95"/>
+      <c r="BD7" s="95"/>
+      <c r="BE7" s="95"/>
+      <c r="BF7" s="95"/>
+      <c r="BG7" s="95"/>
+      <c r="BH7" s="95"/>
+      <c r="BI7" s="95"/>
+      <c r="BJ7" s="95"/>
+      <c r="BK7" s="96"/>
+      <c r="BL7" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="BM7" s="100"/>
-      <c r="BN7" s="100"/>
-      <c r="BO7" s="100"/>
-      <c r="BP7" s="100"/>
-      <c r="BQ7" s="100"/>
-      <c r="BR7" s="100"/>
-      <c r="BS7" s="100"/>
-      <c r="BT7" s="100"/>
-      <c r="BU7" s="101"/>
-      <c r="BV7" s="99" t="s">
+      <c r="BM7" s="95"/>
+      <c r="BN7" s="95"/>
+      <c r="BO7" s="95"/>
+      <c r="BP7" s="95"/>
+      <c r="BQ7" s="95"/>
+      <c r="BR7" s="95"/>
+      <c r="BS7" s="95"/>
+      <c r="BT7" s="95"/>
+      <c r="BU7" s="96"/>
+      <c r="BV7" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="BW7" s="100"/>
-      <c r="BX7" s="100"/>
-      <c r="BY7" s="100"/>
-      <c r="BZ7" s="100"/>
-      <c r="CA7" s="100"/>
-      <c r="CB7" s="100"/>
-      <c r="CC7" s="100"/>
-      <c r="CD7" s="100"/>
-      <c r="CE7" s="101"/>
-      <c r="CF7" s="99" t="s">
+      <c r="BW7" s="95"/>
+      <c r="BX7" s="95"/>
+      <c r="BY7" s="95"/>
+      <c r="BZ7" s="95"/>
+      <c r="CA7" s="95"/>
+      <c r="CB7" s="95"/>
+      <c r="CC7" s="95"/>
+      <c r="CD7" s="95"/>
+      <c r="CE7" s="96"/>
+      <c r="CF7" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="CG7" s="100"/>
-      <c r="CH7" s="100"/>
-      <c r="CI7" s="100"/>
-      <c r="CJ7" s="100"/>
-      <c r="CK7" s="100"/>
-      <c r="CL7" s="100"/>
-      <c r="CM7" s="100"/>
-      <c r="CN7" s="100"/>
-      <c r="CO7" s="101"/>
-      <c r="CP7" s="99" t="s">
+      <c r="CG7" s="95"/>
+      <c r="CH7" s="95"/>
+      <c r="CI7" s="95"/>
+      <c r="CJ7" s="95"/>
+      <c r="CK7" s="95"/>
+      <c r="CL7" s="95"/>
+      <c r="CM7" s="95"/>
+      <c r="CN7" s="95"/>
+      <c r="CO7" s="96"/>
+      <c r="CP7" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="CQ7" s="100"/>
-      <c r="CR7" s="100"/>
-      <c r="CS7" s="100"/>
-      <c r="CT7" s="100"/>
-      <c r="CU7" s="100"/>
-      <c r="CV7" s="100"/>
-      <c r="CW7" s="100"/>
-      <c r="CX7" s="100"/>
-      <c r="CY7" s="101"/>
-      <c r="CZ7" s="99" t="s">
+      <c r="CQ7" s="95"/>
+      <c r="CR7" s="95"/>
+      <c r="CS7" s="95"/>
+      <c r="CT7" s="95"/>
+      <c r="CU7" s="95"/>
+      <c r="CV7" s="95"/>
+      <c r="CW7" s="95"/>
+      <c r="CX7" s="95"/>
+      <c r="CY7" s="96"/>
+      <c r="CZ7" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="DA7" s="100"/>
-      <c r="DB7" s="100"/>
-      <c r="DC7" s="100"/>
-      <c r="DD7" s="100"/>
-      <c r="DE7" s="100"/>
-      <c r="DF7" s="100"/>
-      <c r="DG7" s="100"/>
-      <c r="DH7" s="100"/>
-      <c r="DI7" s="101"/>
-      <c r="DJ7" s="99" t="s">
+      <c r="DA7" s="95"/>
+      <c r="DB7" s="95"/>
+      <c r="DC7" s="95"/>
+      <c r="DD7" s="95"/>
+      <c r="DE7" s="95"/>
+      <c r="DF7" s="95"/>
+      <c r="DG7" s="95"/>
+      <c r="DH7" s="95"/>
+      <c r="DI7" s="96"/>
+      <c r="DJ7" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="DK7" s="100"/>
-      <c r="DL7" s="100"/>
-      <c r="DM7" s="100"/>
-      <c r="DN7" s="100"/>
-      <c r="DO7" s="100"/>
-      <c r="DP7" s="100"/>
-      <c r="DQ7" s="100"/>
-      <c r="DR7" s="100"/>
-      <c r="DS7" s="101"/>
+      <c r="DK7" s="95"/>
+      <c r="DL7" s="95"/>
+      <c r="DM7" s="95"/>
+      <c r="DN7" s="95"/>
+      <c r="DO7" s="95"/>
+      <c r="DP7" s="95"/>
+      <c r="DQ7" s="95"/>
+      <c r="DR7" s="95"/>
+      <c r="DS7" s="96"/>
     </row>
     <row r="8" spans="1:123" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="107"/>
-      <c r="B8" s="108"/>
+      <c r="A8" s="112"/>
+      <c r="B8" s="113"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="90" t="s">
+      <c r="D8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="93" t="s">
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="90" t="s">
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="91"/>
-      <c r="P8" s="91"/>
-      <c r="Q8" s="91"/>
-      <c r="R8" s="92"/>
-      <c r="S8" s="93" t="s">
+      <c r="O8" s="98"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="99"/>
+      <c r="S8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="T8" s="92"/>
-      <c r="U8" s="92"/>
-      <c r="V8" s="92"/>
-      <c r="W8" s="94"/>
-      <c r="X8" s="90" t="s">
+      <c r="T8" s="99"/>
+      <c r="U8" s="99"/>
+      <c r="V8" s="99"/>
+      <c r="W8" s="101"/>
+      <c r="X8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="Y8" s="91"/>
-      <c r="Z8" s="91"/>
-      <c r="AA8" s="91"/>
-      <c r="AB8" s="92"/>
-      <c r="AC8" s="93" t="s">
+      <c r="Y8" s="98"/>
+      <c r="Z8" s="98"/>
+      <c r="AA8" s="98"/>
+      <c r="AB8" s="99"/>
+      <c r="AC8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="AD8" s="92"/>
-      <c r="AE8" s="92"/>
-      <c r="AF8" s="92"/>
-      <c r="AG8" s="94"/>
-      <c r="AH8" s="90" t="s">
+      <c r="AD8" s="99"/>
+      <c r="AE8" s="99"/>
+      <c r="AF8" s="99"/>
+      <c r="AG8" s="101"/>
+      <c r="AH8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="AI8" s="91"/>
-      <c r="AJ8" s="91"/>
-      <c r="AK8" s="91"/>
-      <c r="AL8" s="92"/>
-      <c r="AM8" s="93" t="s">
+      <c r="AI8" s="98"/>
+      <c r="AJ8" s="98"/>
+      <c r="AK8" s="98"/>
+      <c r="AL8" s="99"/>
+      <c r="AM8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="AN8" s="92"/>
-      <c r="AO8" s="92"/>
-      <c r="AP8" s="92"/>
-      <c r="AQ8" s="94"/>
-      <c r="AR8" s="90" t="s">
+      <c r="AN8" s="99"/>
+      <c r="AO8" s="99"/>
+      <c r="AP8" s="99"/>
+      <c r="AQ8" s="101"/>
+      <c r="AR8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="AS8" s="91"/>
-      <c r="AT8" s="91"/>
-      <c r="AU8" s="91"/>
-      <c r="AV8" s="92"/>
-      <c r="AW8" s="93" t="s">
+      <c r="AS8" s="98"/>
+      <c r="AT8" s="98"/>
+      <c r="AU8" s="98"/>
+      <c r="AV8" s="99"/>
+      <c r="AW8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="AX8" s="92"/>
-      <c r="AY8" s="92"/>
-      <c r="AZ8" s="92"/>
-      <c r="BA8" s="94"/>
-      <c r="BB8" s="90" t="s">
+      <c r="AX8" s="99"/>
+      <c r="AY8" s="99"/>
+      <c r="AZ8" s="99"/>
+      <c r="BA8" s="101"/>
+      <c r="BB8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="BC8" s="91"/>
-      <c r="BD8" s="91"/>
-      <c r="BE8" s="91"/>
-      <c r="BF8" s="92"/>
-      <c r="BG8" s="93" t="s">
+      <c r="BC8" s="98"/>
+      <c r="BD8" s="98"/>
+      <c r="BE8" s="98"/>
+      <c r="BF8" s="99"/>
+      <c r="BG8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="BH8" s="92"/>
-      <c r="BI8" s="92"/>
-      <c r="BJ8" s="92"/>
-      <c r="BK8" s="94"/>
-      <c r="BL8" s="90" t="s">
+      <c r="BH8" s="99"/>
+      <c r="BI8" s="99"/>
+      <c r="BJ8" s="99"/>
+      <c r="BK8" s="101"/>
+      <c r="BL8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="BM8" s="91"/>
-      <c r="BN8" s="91"/>
-      <c r="BO8" s="91"/>
-      <c r="BP8" s="92"/>
-      <c r="BQ8" s="93" t="s">
+      <c r="BM8" s="98"/>
+      <c r="BN8" s="98"/>
+      <c r="BO8" s="98"/>
+      <c r="BP8" s="99"/>
+      <c r="BQ8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="BR8" s="92"/>
-      <c r="BS8" s="92"/>
-      <c r="BT8" s="92"/>
-      <c r="BU8" s="94"/>
-      <c r="BV8" s="90" t="s">
+      <c r="BR8" s="99"/>
+      <c r="BS8" s="99"/>
+      <c r="BT8" s="99"/>
+      <c r="BU8" s="101"/>
+      <c r="BV8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="BW8" s="91"/>
-      <c r="BX8" s="91"/>
-      <c r="BY8" s="91"/>
-      <c r="BZ8" s="92"/>
-      <c r="CA8" s="93" t="s">
+      <c r="BW8" s="98"/>
+      <c r="BX8" s="98"/>
+      <c r="BY8" s="98"/>
+      <c r="BZ8" s="99"/>
+      <c r="CA8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="CB8" s="92"/>
-      <c r="CC8" s="92"/>
-      <c r="CD8" s="92"/>
-      <c r="CE8" s="94"/>
-      <c r="CF8" s="90" t="s">
+      <c r="CB8" s="99"/>
+      <c r="CC8" s="99"/>
+      <c r="CD8" s="99"/>
+      <c r="CE8" s="101"/>
+      <c r="CF8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="CG8" s="91"/>
-      <c r="CH8" s="91"/>
-      <c r="CI8" s="91"/>
-      <c r="CJ8" s="92"/>
-      <c r="CK8" s="93" t="s">
+      <c r="CG8" s="98"/>
+      <c r="CH8" s="98"/>
+      <c r="CI8" s="98"/>
+      <c r="CJ8" s="99"/>
+      <c r="CK8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="CL8" s="92"/>
-      <c r="CM8" s="92"/>
-      <c r="CN8" s="92"/>
-      <c r="CO8" s="94"/>
-      <c r="CP8" s="90" t="s">
+      <c r="CL8" s="99"/>
+      <c r="CM8" s="99"/>
+      <c r="CN8" s="99"/>
+      <c r="CO8" s="101"/>
+      <c r="CP8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="CQ8" s="91"/>
-      <c r="CR8" s="91"/>
-      <c r="CS8" s="91"/>
-      <c r="CT8" s="92"/>
-      <c r="CU8" s="93" t="s">
+      <c r="CQ8" s="98"/>
+      <c r="CR8" s="98"/>
+      <c r="CS8" s="98"/>
+      <c r="CT8" s="99"/>
+      <c r="CU8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="CV8" s="92"/>
-      <c r="CW8" s="92"/>
-      <c r="CX8" s="92"/>
-      <c r="CY8" s="94"/>
-      <c r="CZ8" s="90" t="s">
+      <c r="CV8" s="99"/>
+      <c r="CW8" s="99"/>
+      <c r="CX8" s="99"/>
+      <c r="CY8" s="101"/>
+      <c r="CZ8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="DA8" s="91"/>
-      <c r="DB8" s="91"/>
-      <c r="DC8" s="91"/>
-      <c r="DD8" s="92"/>
-      <c r="DE8" s="93" t="s">
+      <c r="DA8" s="98"/>
+      <c r="DB8" s="98"/>
+      <c r="DC8" s="98"/>
+      <c r="DD8" s="99"/>
+      <c r="DE8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="DF8" s="92"/>
-      <c r="DG8" s="92"/>
-      <c r="DH8" s="92"/>
-      <c r="DI8" s="94"/>
-      <c r="DJ8" s="90" t="s">
+      <c r="DF8" s="99"/>
+      <c r="DG8" s="99"/>
+      <c r="DH8" s="99"/>
+      <c r="DI8" s="101"/>
+      <c r="DJ8" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="DK8" s="91"/>
-      <c r="DL8" s="91"/>
-      <c r="DM8" s="91"/>
-      <c r="DN8" s="92"/>
-      <c r="DO8" s="93" t="s">
+      <c r="DK8" s="98"/>
+      <c r="DL8" s="98"/>
+      <c r="DM8" s="98"/>
+      <c r="DN8" s="99"/>
+      <c r="DO8" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="DP8" s="92"/>
-      <c r="DQ8" s="92"/>
-      <c r="DR8" s="92"/>
-      <c r="DS8" s="94"/>
+      <c r="DP8" s="99"/>
+      <c r="DQ8" s="99"/>
+      <c r="DR8" s="99"/>
+      <c r="DS8" s="101"/>
     </row>
     <row r="9" spans="1:123" s="10" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
@@ -1980,7 +1982,7 @@
       <c r="DS9" s="21"/>
     </row>
     <row r="10" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="102">
+      <c r="A10" s="107">
         <v>0</v>
       </c>
       <c r="B10" s="22" t="s">
@@ -2132,7 +2134,7 @@
       <c r="DS10" s="42"/>
     </row>
     <row r="11" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="104"/>
+      <c r="A11" s="109"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25">
         <f>COUNTIF(D11:DS11, "C")</f>
@@ -2274,7 +2276,7 @@
       <c r="DS11" s="50"/>
     </row>
     <row r="12" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="102">
+      <c r="A12" s="107">
         <v>1</v>
       </c>
       <c r="B12" s="22" t="s">
@@ -2424,7 +2426,7 @@
       <c r="DS12" s="42"/>
     </row>
     <row r="13" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="104"/>
+      <c r="A13" s="109"/>
       <c r="B13" s="26"/>
       <c r="C13" s="25">
         <f>COUNTIF(D13:DS13, "C")</f>
@@ -2558,7 +2560,7 @@
       <c r="DS13" s="50"/>
     </row>
     <row r="14" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="109">
+      <c r="A14" s="114">
         <v>2</v>
       </c>
       <c r="B14" s="22" t="s">
@@ -2726,11 +2728,11 @@
       <c r="DS14" s="40"/>
     </row>
     <row r="15" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="104"/>
+      <c r="A15" s="109"/>
       <c r="B15" s="26"/>
       <c r="C15" s="25">
         <f>COUNTIF(D15:DS15, "C")</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="44"/>
@@ -2885,8 +2887,12 @@
       <c r="DB15" s="45"/>
       <c r="DC15" s="45"/>
       <c r="DD15" s="46"/>
-      <c r="DE15" s="46"/>
-      <c r="DF15" s="46"/>
+      <c r="DE15" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="DF15" s="46" t="s">
+        <v>14</v>
+      </c>
       <c r="DG15" s="46"/>
       <c r="DH15" s="46"/>
       <c r="DI15" s="47"/>
@@ -2902,7 +2908,7 @@
       <c r="DS15" s="50"/>
     </row>
     <row r="16" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="102">
+      <c r="A16" s="107">
         <v>3</v>
       </c>
       <c r="B16" s="22" t="s">
@@ -3042,11 +3048,11 @@
       <c r="DS16" s="42"/>
     </row>
     <row r="17" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104"/>
+      <c r="A17" s="109"/>
       <c r="B17" s="27"/>
       <c r="C17" s="25">
         <f>COUNTIF(D17:DS17, "C")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="44"/>
@@ -3138,12 +3144,24 @@
       <c r="CM17" s="84"/>
       <c r="CN17" s="84"/>
       <c r="CO17" s="85"/>
-      <c r="CP17" s="48"/>
-      <c r="CQ17" s="45"/>
-      <c r="CR17" s="45"/>
-      <c r="CS17" s="45"/>
-      <c r="CT17" s="46"/>
-      <c r="CU17" s="46"/>
+      <c r="CP17" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="CQ17" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="CR17" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="CS17" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="CT17" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="CU17" s="46" t="s">
+        <v>14</v>
+      </c>
       <c r="CV17" s="46"/>
       <c r="CW17" s="46"/>
       <c r="CX17" s="46"/>
@@ -3170,7 +3188,7 @@
       <c r="DS17" s="50"/>
     </row>
     <row r="18" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="102">
+      <c r="A18" s="107">
         <v>4</v>
       </c>
       <c r="B18" s="22" t="s">
@@ -3324,11 +3342,11 @@
       <c r="DS18" s="42"/>
     </row>
     <row r="19" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="104"/>
+      <c r="A19" s="109"/>
       <c r="B19" s="27"/>
       <c r="C19" s="25">
         <f>COUNTIF(D19:DS19, "C")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D19" s="43"/>
       <c r="E19" s="44"/>
@@ -3460,8 +3478,12 @@
       <c r="CY19" s="50"/>
       <c r="CZ19" s="48"/>
       <c r="DA19" s="45"/>
-      <c r="DB19" s="45"/>
-      <c r="DC19" s="45"/>
+      <c r="DB19" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="DC19" s="45" t="s">
+        <v>14</v>
+      </c>
       <c r="DD19" s="46"/>
       <c r="DE19" s="46"/>
       <c r="DF19" s="46"/>
@@ -3480,7 +3502,7 @@
       <c r="DS19" s="50"/>
     </row>
     <row r="20" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="102">
+      <c r="A20" s="107">
         <v>5</v>
       </c>
       <c r="B20" s="22" t="s">
@@ -3634,11 +3656,11 @@
       <c r="DS20" s="42"/>
     </row>
     <row r="21" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="104"/>
+      <c r="A21" s="109"/>
       <c r="B21" s="27"/>
       <c r="C21" s="25">
         <f>COUNTIF(D21:DS21, "C")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" s="43"/>
       <c r="E21" s="44"/>
@@ -3760,7 +3782,9 @@
       <c r="DA21" s="45"/>
       <c r="DB21" s="45"/>
       <c r="DC21" s="45"/>
-      <c r="DD21" s="46"/>
+      <c r="DD21" s="46" t="s">
+        <v>14</v>
+      </c>
       <c r="DE21" s="46"/>
       <c r="DF21" s="46"/>
       <c r="DG21" s="46"/>
@@ -3778,7 +3802,7 @@
       <c r="DS21" s="50"/>
     </row>
     <row r="22" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="102">
+      <c r="A22" s="107">
         <v>6</v>
       </c>
       <c r="B22" s="22" t="s">
@@ -3922,11 +3946,11 @@
       <c r="DS22" s="42"/>
     </row>
     <row r="23" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="104"/>
+      <c r="A23" s="109"/>
       <c r="B23" s="27"/>
       <c r="C23" s="25">
         <f>COUNTIF(D23:DS23, "C")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D23" s="43"/>
       <c r="E23" s="44"/>
@@ -4024,12 +4048,20 @@
       <c r="CS23" s="45"/>
       <c r="CT23" s="46"/>
       <c r="CU23" s="46"/>
-      <c r="CV23" s="46"/>
-      <c r="CW23" s="46"/>
+      <c r="CV23" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="CW23" s="46" t="s">
+        <v>14</v>
+      </c>
       <c r="CX23" s="46"/>
       <c r="CY23" s="50"/>
-      <c r="CZ23" s="48"/>
-      <c r="DA23" s="45"/>
+      <c r="CZ23" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="DA23" s="45" t="s">
+        <v>14</v>
+      </c>
       <c r="DB23" s="45"/>
       <c r="DC23" s="45"/>
       <c r="DD23" s="46"/>
@@ -4050,7 +4082,7 @@
       <c r="DS23" s="50"/>
     </row>
     <row r="24" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="102">
+      <c r="A24" s="107">
         <v>7</v>
       </c>
       <c r="B24" s="22"/>
@@ -4180,7 +4212,7 @@
       <c r="DS24" s="42"/>
     </row>
     <row r="25" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="104"/>
+      <c r="A25" s="109"/>
       <c r="B25" s="27"/>
       <c r="C25" s="25">
         <f>COUNTIF(D25:DS25, "C")</f>
@@ -4308,7 +4340,7 @@
       <c r="DS25" s="50"/>
     </row>
     <row r="26" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="102">
+      <c r="A26" s="107">
         <v>8</v>
       </c>
       <c r="B26" s="22" t="s">
@@ -4468,11 +4500,11 @@
       <c r="DS26" s="42"/>
     </row>
     <row r="27" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="104"/>
+      <c r="A27" s="109"/>
       <c r="B27" s="27"/>
       <c r="C27" s="25">
         <f>COUNTIF(D27:DS27, "C")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" s="43"/>
       <c r="E27" s="44"/>
@@ -4576,7 +4608,9 @@
       <c r="CU27" s="46"/>
       <c r="CV27" s="46"/>
       <c r="CW27" s="46"/>
-      <c r="CX27" s="46"/>
+      <c r="CX27" s="46" t="s">
+        <v>14</v>
+      </c>
       <c r="CY27" s="50"/>
       <c r="CZ27" s="48"/>
       <c r="DA27" s="45"/>
@@ -4600,7 +4634,7 @@
       <c r="DS27" s="50"/>
     </row>
     <row r="28" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="102"/>
+      <c r="A28" s="107"/>
       <c r="B28" s="29" t="s">
         <v>5</v>
       </c>
@@ -4730,13 +4764,13 @@
       <c r="DS28" s="42"/>
     </row>
     <row r="29" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="103"/>
+      <c r="A29" s="108"/>
       <c r="B29" s="30" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="31">
         <f>SUM(C11,C13,C15,C17,C19,C21,C23,C25,C27)</f>
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="D29" s="51"/>
       <c r="E29" s="51"/>
@@ -5058,21 +5092,41 @@
     <row r="35" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="CZ6:DI6"/>
-    <mergeCell ref="DJ6:DS6"/>
-    <mergeCell ref="CZ7:DI7"/>
-    <mergeCell ref="DJ7:DS7"/>
-    <mergeCell ref="CZ8:DD8"/>
-    <mergeCell ref="DE8:DI8"/>
-    <mergeCell ref="DJ8:DN8"/>
-    <mergeCell ref="DO8:DS8"/>
-    <mergeCell ref="BH4:BI4"/>
-    <mergeCell ref="N6:W6"/>
-    <mergeCell ref="N7:W7"/>
-    <mergeCell ref="X6:AG6"/>
-    <mergeCell ref="AH6:AQ6"/>
-    <mergeCell ref="X7:AG7"/>
-    <mergeCell ref="AH7:AQ7"/>
+    <mergeCell ref="CF8:CJ8"/>
+    <mergeCell ref="CK8:CO8"/>
+    <mergeCell ref="CP8:CT8"/>
+    <mergeCell ref="CU8:CY8"/>
+    <mergeCell ref="CF6:CO6"/>
+    <mergeCell ref="CP6:CY6"/>
+    <mergeCell ref="CF7:CO7"/>
+    <mergeCell ref="CP7:CY7"/>
+    <mergeCell ref="BL6:BU6"/>
+    <mergeCell ref="BV6:CE6"/>
+    <mergeCell ref="BL7:BU7"/>
+    <mergeCell ref="BV7:CE7"/>
+    <mergeCell ref="BL8:BP8"/>
+    <mergeCell ref="BQ8:BU8"/>
+    <mergeCell ref="BV8:BZ8"/>
+    <mergeCell ref="CA8:CE8"/>
+    <mergeCell ref="BG8:BK8"/>
+    <mergeCell ref="AR6:BA6"/>
+    <mergeCell ref="BB6:BK6"/>
+    <mergeCell ref="AR7:BA7"/>
+    <mergeCell ref="BB7:BK7"/>
+    <mergeCell ref="AR8:AV8"/>
+    <mergeCell ref="AW8:BA8"/>
+    <mergeCell ref="BB8:BF8"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A6:B8"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="N8:R8"/>
     <mergeCell ref="S8:W8"/>
     <mergeCell ref="AV2:BC2"/>
@@ -5087,41 +5141,21 @@
     <mergeCell ref="AN2:AT2"/>
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="AV4:BC4"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A6:B8"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="BG8:BK8"/>
-    <mergeCell ref="AR6:BA6"/>
-    <mergeCell ref="BB6:BK6"/>
-    <mergeCell ref="AR7:BA7"/>
-    <mergeCell ref="BB7:BK7"/>
-    <mergeCell ref="AR8:AV8"/>
-    <mergeCell ref="AW8:BA8"/>
-    <mergeCell ref="BB8:BF8"/>
-    <mergeCell ref="BL6:BU6"/>
-    <mergeCell ref="BV6:CE6"/>
-    <mergeCell ref="BL7:BU7"/>
-    <mergeCell ref="BV7:CE7"/>
-    <mergeCell ref="BL8:BP8"/>
-    <mergeCell ref="BQ8:BU8"/>
-    <mergeCell ref="BV8:BZ8"/>
-    <mergeCell ref="CA8:CE8"/>
-    <mergeCell ref="CF8:CJ8"/>
-    <mergeCell ref="CK8:CO8"/>
-    <mergeCell ref="CP8:CT8"/>
-    <mergeCell ref="CU8:CY8"/>
-    <mergeCell ref="CF6:CO6"/>
-    <mergeCell ref="CP6:CY6"/>
-    <mergeCell ref="CF7:CO7"/>
-    <mergeCell ref="CP7:CY7"/>
+    <mergeCell ref="BH4:BI4"/>
+    <mergeCell ref="N6:W6"/>
+    <mergeCell ref="N7:W7"/>
+    <mergeCell ref="X6:AG6"/>
+    <mergeCell ref="AH6:AQ6"/>
+    <mergeCell ref="X7:AG7"/>
+    <mergeCell ref="AH7:AQ7"/>
+    <mergeCell ref="CZ6:DI6"/>
+    <mergeCell ref="DJ6:DS6"/>
+    <mergeCell ref="CZ7:DI7"/>
+    <mergeCell ref="DJ7:DS7"/>
+    <mergeCell ref="CZ8:DD8"/>
+    <mergeCell ref="DE8:DI8"/>
+    <mergeCell ref="DJ8:DN8"/>
+    <mergeCell ref="DO8:DS8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D10:CY29">

</xml_diff>

<commit_message>
Update plan and journal
</commit_message>
<xml_diff>
--- a/doc/Pianificazione.xlsx
+++ b/doc/Pianificazione.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="28">
   <si>
     <t>ATTIVITÀ</t>
   </si>
@@ -782,6 +782,21 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -802,36 +817,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -857,11 +842,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color theme="4" tint="0.39994506668294322"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.39994506668294322"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="4" tint="0.39994506668294322"/>
@@ -1187,7 +1207,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="CQ32" sqref="CQ32"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1240,23 +1260,23 @@
       <c r="AI2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AN2" s="104">
+      <c r="AN2" s="111">
         <v>43202</v>
       </c>
-      <c r="AO2" s="104"/>
-      <c r="AP2" s="104"/>
-      <c r="AQ2" s="104"/>
-      <c r="AR2" s="104"/>
-      <c r="AS2" s="104"/>
-      <c r="AT2" s="104"/>
-      <c r="AV2" s="103"/>
-      <c r="AW2" s="103"/>
-      <c r="AX2" s="103"/>
-      <c r="AY2" s="103"/>
-      <c r="AZ2" s="103"/>
-      <c r="BA2" s="103"/>
-      <c r="BB2" s="103"/>
-      <c r="BC2" s="103"/>
+      <c r="AO2" s="111"/>
+      <c r="AP2" s="111"/>
+      <c r="AQ2" s="111"/>
+      <c r="AR2" s="111"/>
+      <c r="AS2" s="111"/>
+      <c r="AT2" s="111"/>
+      <c r="AV2" s="110"/>
+      <c r="AW2" s="110"/>
+      <c r="AX2" s="110"/>
+      <c r="AY2" s="110"/>
+      <c r="AZ2" s="110"/>
+      <c r="BA2" s="110"/>
+      <c r="BB2" s="110"/>
+      <c r="BC2" s="110"/>
     </row>
     <row r="3" spans="1:123" s="1" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
@@ -1356,501 +1376,501 @@
       <c r="AI4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AN4" s="105">
+      <c r="AN4" s="112">
         <v>43235</v>
       </c>
-      <c r="AO4" s="106"/>
-      <c r="AP4" s="106"/>
-      <c r="AQ4" s="106"/>
-      <c r="AR4" s="106"/>
-      <c r="AS4" s="106"/>
-      <c r="AT4" s="106"/>
-      <c r="AV4" s="103"/>
-      <c r="AW4" s="103"/>
-      <c r="AX4" s="103"/>
-      <c r="AY4" s="103"/>
-      <c r="AZ4" s="103"/>
-      <c r="BA4" s="103"/>
-      <c r="BB4" s="103"/>
-      <c r="BC4" s="103"/>
-      <c r="BH4" s="102"/>
-      <c r="BI4" s="102"/>
+      <c r="AO4" s="113"/>
+      <c r="AP4" s="113"/>
+      <c r="AQ4" s="113"/>
+      <c r="AR4" s="113"/>
+      <c r="AS4" s="113"/>
+      <c r="AT4" s="113"/>
+      <c r="AV4" s="110"/>
+      <c r="AW4" s="110"/>
+      <c r="AX4" s="110"/>
+      <c r="AY4" s="110"/>
+      <c r="AZ4" s="110"/>
+      <c r="BA4" s="110"/>
+      <c r="BB4" s="110"/>
+      <c r="BC4" s="110"/>
+      <c r="BH4" s="114"/>
+      <c r="BI4" s="114"/>
     </row>
     <row r="5" spans="1:123" s="1" customFormat="1" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:123" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="110"/>
-      <c r="B6" s="111"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="106"/>
       <c r="C6" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="90">
+      <c r="D6" s="95">
         <v>43202</v>
       </c>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="90">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="95">
         <v>43203</v>
       </c>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="92"/>
-      <c r="T6" s="92"/>
-      <c r="U6" s="92"/>
-      <c r="V6" s="92"/>
-      <c r="W6" s="93"/>
-      <c r="X6" s="90">
+      <c r="O6" s="96"/>
+      <c r="P6" s="96"/>
+      <c r="Q6" s="96"/>
+      <c r="R6" s="97"/>
+      <c r="S6" s="97"/>
+      <c r="T6" s="97"/>
+      <c r="U6" s="97"/>
+      <c r="V6" s="97"/>
+      <c r="W6" s="98"/>
+      <c r="X6" s="95">
         <v>43206</v>
       </c>
-      <c r="Y6" s="91"/>
-      <c r="Z6" s="91"/>
-      <c r="AA6" s="91"/>
-      <c r="AB6" s="92"/>
-      <c r="AC6" s="92"/>
-      <c r="AD6" s="92"/>
-      <c r="AE6" s="92"/>
-      <c r="AF6" s="92"/>
-      <c r="AG6" s="93"/>
-      <c r="AH6" s="90">
+      <c r="Y6" s="96"/>
+      <c r="Z6" s="96"/>
+      <c r="AA6" s="96"/>
+      <c r="AB6" s="97"/>
+      <c r="AC6" s="97"/>
+      <c r="AD6" s="97"/>
+      <c r="AE6" s="97"/>
+      <c r="AF6" s="97"/>
+      <c r="AG6" s="98"/>
+      <c r="AH6" s="95">
         <v>43207</v>
       </c>
-      <c r="AI6" s="91"/>
-      <c r="AJ6" s="91"/>
-      <c r="AK6" s="91"/>
-      <c r="AL6" s="92"/>
-      <c r="AM6" s="92"/>
-      <c r="AN6" s="92"/>
-      <c r="AO6" s="92"/>
-      <c r="AP6" s="92"/>
-      <c r="AQ6" s="93"/>
-      <c r="AR6" s="90">
+      <c r="AI6" s="96"/>
+      <c r="AJ6" s="96"/>
+      <c r="AK6" s="96"/>
+      <c r="AL6" s="97"/>
+      <c r="AM6" s="97"/>
+      <c r="AN6" s="97"/>
+      <c r="AO6" s="97"/>
+      <c r="AP6" s="97"/>
+      <c r="AQ6" s="98"/>
+      <c r="AR6" s="95">
         <v>43216</v>
       </c>
-      <c r="AS6" s="91"/>
-      <c r="AT6" s="91"/>
-      <c r="AU6" s="91"/>
-      <c r="AV6" s="92"/>
-      <c r="AW6" s="92"/>
-      <c r="AX6" s="92"/>
-      <c r="AY6" s="92"/>
-      <c r="AZ6" s="92"/>
-      <c r="BA6" s="93"/>
-      <c r="BB6" s="90">
+      <c r="AS6" s="96"/>
+      <c r="AT6" s="96"/>
+      <c r="AU6" s="96"/>
+      <c r="AV6" s="97"/>
+      <c r="AW6" s="97"/>
+      <c r="AX6" s="97"/>
+      <c r="AY6" s="97"/>
+      <c r="AZ6" s="97"/>
+      <c r="BA6" s="98"/>
+      <c r="BB6" s="95">
         <v>43217</v>
       </c>
-      <c r="BC6" s="91"/>
-      <c r="BD6" s="91"/>
-      <c r="BE6" s="91"/>
-      <c r="BF6" s="92"/>
-      <c r="BG6" s="92"/>
-      <c r="BH6" s="92"/>
-      <c r="BI6" s="92"/>
-      <c r="BJ6" s="92"/>
-      <c r="BK6" s="93"/>
-      <c r="BL6" s="90">
+      <c r="BC6" s="96"/>
+      <c r="BD6" s="96"/>
+      <c r="BE6" s="96"/>
+      <c r="BF6" s="97"/>
+      <c r="BG6" s="97"/>
+      <c r="BH6" s="97"/>
+      <c r="BI6" s="97"/>
+      <c r="BJ6" s="97"/>
+      <c r="BK6" s="98"/>
+      <c r="BL6" s="95">
         <v>43220</v>
       </c>
-      <c r="BM6" s="91"/>
-      <c r="BN6" s="91"/>
-      <c r="BO6" s="91"/>
-      <c r="BP6" s="92"/>
-      <c r="BQ6" s="92"/>
-      <c r="BR6" s="92"/>
-      <c r="BS6" s="92"/>
-      <c r="BT6" s="92"/>
-      <c r="BU6" s="93"/>
-      <c r="BV6" s="90">
+      <c r="BM6" s="96"/>
+      <c r="BN6" s="96"/>
+      <c r="BO6" s="96"/>
+      <c r="BP6" s="97"/>
+      <c r="BQ6" s="97"/>
+      <c r="BR6" s="97"/>
+      <c r="BS6" s="97"/>
+      <c r="BT6" s="97"/>
+      <c r="BU6" s="98"/>
+      <c r="BV6" s="95">
         <v>43221</v>
       </c>
-      <c r="BW6" s="91"/>
-      <c r="BX6" s="91"/>
-      <c r="BY6" s="91"/>
-      <c r="BZ6" s="92"/>
-      <c r="CA6" s="92"/>
-      <c r="CB6" s="92"/>
-      <c r="CC6" s="92"/>
-      <c r="CD6" s="92"/>
-      <c r="CE6" s="93"/>
-      <c r="CF6" s="90">
+      <c r="BW6" s="96"/>
+      <c r="BX6" s="96"/>
+      <c r="BY6" s="96"/>
+      <c r="BZ6" s="97"/>
+      <c r="CA6" s="97"/>
+      <c r="CB6" s="97"/>
+      <c r="CC6" s="97"/>
+      <c r="CD6" s="97"/>
+      <c r="CE6" s="98"/>
+      <c r="CF6" s="95">
         <v>43230</v>
       </c>
-      <c r="CG6" s="91"/>
-      <c r="CH6" s="91"/>
-      <c r="CI6" s="91"/>
-      <c r="CJ6" s="92"/>
-      <c r="CK6" s="92"/>
-      <c r="CL6" s="92"/>
-      <c r="CM6" s="92"/>
-      <c r="CN6" s="92"/>
-      <c r="CO6" s="93"/>
-      <c r="CP6" s="90">
+      <c r="CG6" s="96"/>
+      <c r="CH6" s="96"/>
+      <c r="CI6" s="96"/>
+      <c r="CJ6" s="97"/>
+      <c r="CK6" s="97"/>
+      <c r="CL6" s="97"/>
+      <c r="CM6" s="97"/>
+      <c r="CN6" s="97"/>
+      <c r="CO6" s="98"/>
+      <c r="CP6" s="95">
         <v>43231</v>
       </c>
-      <c r="CQ6" s="91"/>
-      <c r="CR6" s="91"/>
-      <c r="CS6" s="91"/>
-      <c r="CT6" s="92"/>
-      <c r="CU6" s="92"/>
-      <c r="CV6" s="92"/>
-      <c r="CW6" s="92"/>
-      <c r="CX6" s="92"/>
-      <c r="CY6" s="93"/>
-      <c r="CZ6" s="90">
+      <c r="CQ6" s="96"/>
+      <c r="CR6" s="96"/>
+      <c r="CS6" s="96"/>
+      <c r="CT6" s="97"/>
+      <c r="CU6" s="97"/>
+      <c r="CV6" s="97"/>
+      <c r="CW6" s="97"/>
+      <c r="CX6" s="97"/>
+      <c r="CY6" s="98"/>
+      <c r="CZ6" s="95">
         <v>43234</v>
       </c>
-      <c r="DA6" s="91"/>
-      <c r="DB6" s="91"/>
-      <c r="DC6" s="91"/>
-      <c r="DD6" s="92"/>
-      <c r="DE6" s="92"/>
-      <c r="DF6" s="92"/>
-      <c r="DG6" s="92"/>
-      <c r="DH6" s="92"/>
-      <c r="DI6" s="93"/>
-      <c r="DJ6" s="90">
+      <c r="DA6" s="96"/>
+      <c r="DB6" s="96"/>
+      <c r="DC6" s="96"/>
+      <c r="DD6" s="97"/>
+      <c r="DE6" s="97"/>
+      <c r="DF6" s="97"/>
+      <c r="DG6" s="97"/>
+      <c r="DH6" s="97"/>
+      <c r="DI6" s="98"/>
+      <c r="DJ6" s="95">
         <v>43235</v>
       </c>
-      <c r="DK6" s="91"/>
-      <c r="DL6" s="91"/>
-      <c r="DM6" s="91"/>
-      <c r="DN6" s="92"/>
-      <c r="DO6" s="92"/>
-      <c r="DP6" s="92"/>
-      <c r="DQ6" s="92"/>
-      <c r="DR6" s="92"/>
-      <c r="DS6" s="93"/>
+      <c r="DK6" s="96"/>
+      <c r="DL6" s="96"/>
+      <c r="DM6" s="96"/>
+      <c r="DN6" s="97"/>
+      <c r="DO6" s="97"/>
+      <c r="DP6" s="97"/>
+      <c r="DQ6" s="97"/>
+      <c r="DR6" s="97"/>
+      <c r="DS6" s="98"/>
     </row>
     <row r="7" spans="1:123" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="112"/>
-      <c r="B7" s="113"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="94" t="s">
+      <c r="D7" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="94" t="s">
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="101"/>
+      <c r="N7" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="95"/>
-      <c r="P7" s="95"/>
-      <c r="Q7" s="95"/>
-      <c r="R7" s="95"/>
-      <c r="S7" s="95"/>
-      <c r="T7" s="95"/>
-      <c r="U7" s="95"/>
-      <c r="V7" s="95"/>
-      <c r="W7" s="96"/>
-      <c r="X7" s="94" t="s">
+      <c r="O7" s="100"/>
+      <c r="P7" s="100"/>
+      <c r="Q7" s="100"/>
+      <c r="R7" s="100"/>
+      <c r="S7" s="100"/>
+      <c r="T7" s="100"/>
+      <c r="U7" s="100"/>
+      <c r="V7" s="100"/>
+      <c r="W7" s="101"/>
+      <c r="X7" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="Y7" s="95"/>
-      <c r="Z7" s="95"/>
-      <c r="AA7" s="95"/>
-      <c r="AB7" s="95"/>
-      <c r="AC7" s="95"/>
-      <c r="AD7" s="95"/>
-      <c r="AE7" s="95"/>
-      <c r="AF7" s="95"/>
-      <c r="AG7" s="96"/>
-      <c r="AH7" s="94" t="s">
+      <c r="Y7" s="100"/>
+      <c r="Z7" s="100"/>
+      <c r="AA7" s="100"/>
+      <c r="AB7" s="100"/>
+      <c r="AC7" s="100"/>
+      <c r="AD7" s="100"/>
+      <c r="AE7" s="100"/>
+      <c r="AF7" s="100"/>
+      <c r="AG7" s="101"/>
+      <c r="AH7" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="AI7" s="95"/>
-      <c r="AJ7" s="95"/>
-      <c r="AK7" s="95"/>
-      <c r="AL7" s="95"/>
-      <c r="AM7" s="95"/>
-      <c r="AN7" s="95"/>
-      <c r="AO7" s="95"/>
-      <c r="AP7" s="95"/>
-      <c r="AQ7" s="96"/>
-      <c r="AR7" s="94" t="s">
+      <c r="AI7" s="100"/>
+      <c r="AJ7" s="100"/>
+      <c r="AK7" s="100"/>
+      <c r="AL7" s="100"/>
+      <c r="AM7" s="100"/>
+      <c r="AN7" s="100"/>
+      <c r="AO7" s="100"/>
+      <c r="AP7" s="100"/>
+      <c r="AQ7" s="101"/>
+      <c r="AR7" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="AS7" s="95"/>
-      <c r="AT7" s="95"/>
-      <c r="AU7" s="95"/>
-      <c r="AV7" s="95"/>
-      <c r="AW7" s="95"/>
-      <c r="AX7" s="95"/>
-      <c r="AY7" s="95"/>
-      <c r="AZ7" s="95"/>
-      <c r="BA7" s="96"/>
-      <c r="BB7" s="94" t="s">
+      <c r="AS7" s="100"/>
+      <c r="AT7" s="100"/>
+      <c r="AU7" s="100"/>
+      <c r="AV7" s="100"/>
+      <c r="AW7" s="100"/>
+      <c r="AX7" s="100"/>
+      <c r="AY7" s="100"/>
+      <c r="AZ7" s="100"/>
+      <c r="BA7" s="101"/>
+      <c r="BB7" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="BC7" s="95"/>
-      <c r="BD7" s="95"/>
-      <c r="BE7" s="95"/>
-      <c r="BF7" s="95"/>
-      <c r="BG7" s="95"/>
-      <c r="BH7" s="95"/>
-      <c r="BI7" s="95"/>
-      <c r="BJ7" s="95"/>
-      <c r="BK7" s="96"/>
-      <c r="BL7" s="94" t="s">
+      <c r="BC7" s="100"/>
+      <c r="BD7" s="100"/>
+      <c r="BE7" s="100"/>
+      <c r="BF7" s="100"/>
+      <c r="BG7" s="100"/>
+      <c r="BH7" s="100"/>
+      <c r="BI7" s="100"/>
+      <c r="BJ7" s="100"/>
+      <c r="BK7" s="101"/>
+      <c r="BL7" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="BM7" s="95"/>
-      <c r="BN7" s="95"/>
-      <c r="BO7" s="95"/>
-      <c r="BP7" s="95"/>
-      <c r="BQ7" s="95"/>
-      <c r="BR7" s="95"/>
-      <c r="BS7" s="95"/>
-      <c r="BT7" s="95"/>
-      <c r="BU7" s="96"/>
-      <c r="BV7" s="94" t="s">
+      <c r="BM7" s="100"/>
+      <c r="BN7" s="100"/>
+      <c r="BO7" s="100"/>
+      <c r="BP7" s="100"/>
+      <c r="BQ7" s="100"/>
+      <c r="BR7" s="100"/>
+      <c r="BS7" s="100"/>
+      <c r="BT7" s="100"/>
+      <c r="BU7" s="101"/>
+      <c r="BV7" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="BW7" s="95"/>
-      <c r="BX7" s="95"/>
-      <c r="BY7" s="95"/>
-      <c r="BZ7" s="95"/>
-      <c r="CA7" s="95"/>
-      <c r="CB7" s="95"/>
-      <c r="CC7" s="95"/>
-      <c r="CD7" s="95"/>
-      <c r="CE7" s="96"/>
-      <c r="CF7" s="94" t="s">
+      <c r="BW7" s="100"/>
+      <c r="BX7" s="100"/>
+      <c r="BY7" s="100"/>
+      <c r="BZ7" s="100"/>
+      <c r="CA7" s="100"/>
+      <c r="CB7" s="100"/>
+      <c r="CC7" s="100"/>
+      <c r="CD7" s="100"/>
+      <c r="CE7" s="101"/>
+      <c r="CF7" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="CG7" s="95"/>
-      <c r="CH7" s="95"/>
-      <c r="CI7" s="95"/>
-      <c r="CJ7" s="95"/>
-      <c r="CK7" s="95"/>
-      <c r="CL7" s="95"/>
-      <c r="CM7" s="95"/>
-      <c r="CN7" s="95"/>
-      <c r="CO7" s="96"/>
-      <c r="CP7" s="94" t="s">
+      <c r="CG7" s="100"/>
+      <c r="CH7" s="100"/>
+      <c r="CI7" s="100"/>
+      <c r="CJ7" s="100"/>
+      <c r="CK7" s="100"/>
+      <c r="CL7" s="100"/>
+      <c r="CM7" s="100"/>
+      <c r="CN7" s="100"/>
+      <c r="CO7" s="101"/>
+      <c r="CP7" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="CQ7" s="95"/>
-      <c r="CR7" s="95"/>
-      <c r="CS7" s="95"/>
-      <c r="CT7" s="95"/>
-      <c r="CU7" s="95"/>
-      <c r="CV7" s="95"/>
-      <c r="CW7" s="95"/>
-      <c r="CX7" s="95"/>
-      <c r="CY7" s="96"/>
-      <c r="CZ7" s="94" t="s">
+      <c r="CQ7" s="100"/>
+      <c r="CR7" s="100"/>
+      <c r="CS7" s="100"/>
+      <c r="CT7" s="100"/>
+      <c r="CU7" s="100"/>
+      <c r="CV7" s="100"/>
+      <c r="CW7" s="100"/>
+      <c r="CX7" s="100"/>
+      <c r="CY7" s="101"/>
+      <c r="CZ7" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="DA7" s="95"/>
-      <c r="DB7" s="95"/>
-      <c r="DC7" s="95"/>
-      <c r="DD7" s="95"/>
-      <c r="DE7" s="95"/>
-      <c r="DF7" s="95"/>
-      <c r="DG7" s="95"/>
-      <c r="DH7" s="95"/>
-      <c r="DI7" s="96"/>
-      <c r="DJ7" s="94" t="s">
+      <c r="DA7" s="100"/>
+      <c r="DB7" s="100"/>
+      <c r="DC7" s="100"/>
+      <c r="DD7" s="100"/>
+      <c r="DE7" s="100"/>
+      <c r="DF7" s="100"/>
+      <c r="DG7" s="100"/>
+      <c r="DH7" s="100"/>
+      <c r="DI7" s="101"/>
+      <c r="DJ7" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="DK7" s="95"/>
-      <c r="DL7" s="95"/>
-      <c r="DM7" s="95"/>
-      <c r="DN7" s="95"/>
-      <c r="DO7" s="95"/>
-      <c r="DP7" s="95"/>
-      <c r="DQ7" s="95"/>
-      <c r="DR7" s="95"/>
-      <c r="DS7" s="96"/>
+      <c r="DK7" s="100"/>
+      <c r="DL7" s="100"/>
+      <c r="DM7" s="100"/>
+      <c r="DN7" s="100"/>
+      <c r="DO7" s="100"/>
+      <c r="DP7" s="100"/>
+      <c r="DQ7" s="100"/>
+      <c r="DR7" s="100"/>
+      <c r="DS7" s="101"/>
     </row>
     <row r="8" spans="1:123" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="112"/>
-      <c r="B8" s="113"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="108"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="100" t="s">
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="101"/>
-      <c r="N8" s="97" t="s">
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="98"/>
-      <c r="P8" s="98"/>
-      <c r="Q8" s="98"/>
-      <c r="R8" s="99"/>
-      <c r="S8" s="100" t="s">
+      <c r="O8" s="91"/>
+      <c r="P8" s="91"/>
+      <c r="Q8" s="91"/>
+      <c r="R8" s="92"/>
+      <c r="S8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="T8" s="99"/>
-      <c r="U8" s="99"/>
-      <c r="V8" s="99"/>
-      <c r="W8" s="101"/>
-      <c r="X8" s="97" t="s">
+      <c r="T8" s="92"/>
+      <c r="U8" s="92"/>
+      <c r="V8" s="92"/>
+      <c r="W8" s="94"/>
+      <c r="X8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="Y8" s="98"/>
-      <c r="Z8" s="98"/>
-      <c r="AA8" s="98"/>
-      <c r="AB8" s="99"/>
-      <c r="AC8" s="100" t="s">
+      <c r="Y8" s="91"/>
+      <c r="Z8" s="91"/>
+      <c r="AA8" s="91"/>
+      <c r="AB8" s="92"/>
+      <c r="AC8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="AD8" s="99"/>
-      <c r="AE8" s="99"/>
-      <c r="AF8" s="99"/>
-      <c r="AG8" s="101"/>
-      <c r="AH8" s="97" t="s">
+      <c r="AD8" s="92"/>
+      <c r="AE8" s="92"/>
+      <c r="AF8" s="92"/>
+      <c r="AG8" s="94"/>
+      <c r="AH8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="AI8" s="98"/>
-      <c r="AJ8" s="98"/>
-      <c r="AK8" s="98"/>
-      <c r="AL8" s="99"/>
-      <c r="AM8" s="100" t="s">
+      <c r="AI8" s="91"/>
+      <c r="AJ8" s="91"/>
+      <c r="AK8" s="91"/>
+      <c r="AL8" s="92"/>
+      <c r="AM8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="AN8" s="99"/>
-      <c r="AO8" s="99"/>
-      <c r="AP8" s="99"/>
-      <c r="AQ8" s="101"/>
-      <c r="AR8" s="97" t="s">
+      <c r="AN8" s="92"/>
+      <c r="AO8" s="92"/>
+      <c r="AP8" s="92"/>
+      <c r="AQ8" s="94"/>
+      <c r="AR8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="AS8" s="98"/>
-      <c r="AT8" s="98"/>
-      <c r="AU8" s="98"/>
-      <c r="AV8" s="99"/>
-      <c r="AW8" s="100" t="s">
+      <c r="AS8" s="91"/>
+      <c r="AT8" s="91"/>
+      <c r="AU8" s="91"/>
+      <c r="AV8" s="92"/>
+      <c r="AW8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="AX8" s="99"/>
-      <c r="AY8" s="99"/>
-      <c r="AZ8" s="99"/>
-      <c r="BA8" s="101"/>
-      <c r="BB8" s="97" t="s">
+      <c r="AX8" s="92"/>
+      <c r="AY8" s="92"/>
+      <c r="AZ8" s="92"/>
+      <c r="BA8" s="94"/>
+      <c r="BB8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="BC8" s="98"/>
-      <c r="BD8" s="98"/>
-      <c r="BE8" s="98"/>
-      <c r="BF8" s="99"/>
-      <c r="BG8" s="100" t="s">
+      <c r="BC8" s="91"/>
+      <c r="BD8" s="91"/>
+      <c r="BE8" s="91"/>
+      <c r="BF8" s="92"/>
+      <c r="BG8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="BH8" s="99"/>
-      <c r="BI8" s="99"/>
-      <c r="BJ8" s="99"/>
-      <c r="BK8" s="101"/>
-      <c r="BL8" s="97" t="s">
+      <c r="BH8" s="92"/>
+      <c r="BI8" s="92"/>
+      <c r="BJ8" s="92"/>
+      <c r="BK8" s="94"/>
+      <c r="BL8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="BM8" s="98"/>
-      <c r="BN8" s="98"/>
-      <c r="BO8" s="98"/>
-      <c r="BP8" s="99"/>
-      <c r="BQ8" s="100" t="s">
+      <c r="BM8" s="91"/>
+      <c r="BN8" s="91"/>
+      <c r="BO8" s="91"/>
+      <c r="BP8" s="92"/>
+      <c r="BQ8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="BR8" s="99"/>
-      <c r="BS8" s="99"/>
-      <c r="BT8" s="99"/>
-      <c r="BU8" s="101"/>
-      <c r="BV8" s="97" t="s">
+      <c r="BR8" s="92"/>
+      <c r="BS8" s="92"/>
+      <c r="BT8" s="92"/>
+      <c r="BU8" s="94"/>
+      <c r="BV8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="BW8" s="98"/>
-      <c r="BX8" s="98"/>
-      <c r="BY8" s="98"/>
-      <c r="BZ8" s="99"/>
-      <c r="CA8" s="100" t="s">
+      <c r="BW8" s="91"/>
+      <c r="BX8" s="91"/>
+      <c r="BY8" s="91"/>
+      <c r="BZ8" s="92"/>
+      <c r="CA8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="CB8" s="99"/>
-      <c r="CC8" s="99"/>
-      <c r="CD8" s="99"/>
-      <c r="CE8" s="101"/>
-      <c r="CF8" s="97" t="s">
+      <c r="CB8" s="92"/>
+      <c r="CC8" s="92"/>
+      <c r="CD8" s="92"/>
+      <c r="CE8" s="94"/>
+      <c r="CF8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="CG8" s="98"/>
-      <c r="CH8" s="98"/>
-      <c r="CI8" s="98"/>
-      <c r="CJ8" s="99"/>
-      <c r="CK8" s="100" t="s">
+      <c r="CG8" s="91"/>
+      <c r="CH8" s="91"/>
+      <c r="CI8" s="91"/>
+      <c r="CJ8" s="92"/>
+      <c r="CK8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="CL8" s="99"/>
-      <c r="CM8" s="99"/>
-      <c r="CN8" s="99"/>
-      <c r="CO8" s="101"/>
-      <c r="CP8" s="97" t="s">
+      <c r="CL8" s="92"/>
+      <c r="CM8" s="92"/>
+      <c r="CN8" s="92"/>
+      <c r="CO8" s="94"/>
+      <c r="CP8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="CQ8" s="98"/>
-      <c r="CR8" s="98"/>
-      <c r="CS8" s="98"/>
-      <c r="CT8" s="99"/>
-      <c r="CU8" s="100" t="s">
+      <c r="CQ8" s="91"/>
+      <c r="CR8" s="91"/>
+      <c r="CS8" s="91"/>
+      <c r="CT8" s="92"/>
+      <c r="CU8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="CV8" s="99"/>
-      <c r="CW8" s="99"/>
-      <c r="CX8" s="99"/>
-      <c r="CY8" s="101"/>
-      <c r="CZ8" s="97" t="s">
+      <c r="CV8" s="92"/>
+      <c r="CW8" s="92"/>
+      <c r="CX8" s="92"/>
+      <c r="CY8" s="94"/>
+      <c r="CZ8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="DA8" s="98"/>
-      <c r="DB8" s="98"/>
-      <c r="DC8" s="98"/>
-      <c r="DD8" s="99"/>
-      <c r="DE8" s="100" t="s">
+      <c r="DA8" s="91"/>
+      <c r="DB8" s="91"/>
+      <c r="DC8" s="91"/>
+      <c r="DD8" s="92"/>
+      <c r="DE8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="DF8" s="99"/>
-      <c r="DG8" s="99"/>
-      <c r="DH8" s="99"/>
-      <c r="DI8" s="101"/>
-      <c r="DJ8" s="97" t="s">
+      <c r="DF8" s="92"/>
+      <c r="DG8" s="92"/>
+      <c r="DH8" s="92"/>
+      <c r="DI8" s="94"/>
+      <c r="DJ8" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="DK8" s="98"/>
-      <c r="DL8" s="98"/>
-      <c r="DM8" s="98"/>
-      <c r="DN8" s="99"/>
-      <c r="DO8" s="100" t="s">
+      <c r="DK8" s="91"/>
+      <c r="DL8" s="91"/>
+      <c r="DM8" s="91"/>
+      <c r="DN8" s="92"/>
+      <c r="DO8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="DP8" s="99"/>
-      <c r="DQ8" s="99"/>
-      <c r="DR8" s="99"/>
-      <c r="DS8" s="101"/>
+      <c r="DP8" s="92"/>
+      <c r="DQ8" s="92"/>
+      <c r="DR8" s="92"/>
+      <c r="DS8" s="94"/>
     </row>
     <row r="9" spans="1:123" s="10" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
@@ -1982,7 +2002,7 @@
       <c r="DS9" s="21"/>
     </row>
     <row r="10" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="107">
+      <c r="A10" s="102">
         <v>0</v>
       </c>
       <c r="B10" s="22" t="s">
@@ -2134,16 +2154,18 @@
       <c r="DS10" s="42"/>
     </row>
     <row r="11" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="109"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25">
         <f>COUNTIF(D11:DS11, "C")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="44"/>
       <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
+      <c r="G11" s="45" t="s">
+        <v>14</v>
+      </c>
       <c r="H11" s="46" t="s">
         <v>14</v>
       </c>
@@ -2276,7 +2298,7 @@
       <c r="DS11" s="50"/>
     </row>
     <row r="12" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="107">
+      <c r="A12" s="102">
         <v>1</v>
       </c>
       <c r="B12" s="22" t="s">
@@ -2426,7 +2448,7 @@
       <c r="DS12" s="42"/>
     </row>
     <row r="13" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="109"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="26"/>
       <c r="C13" s="25">
         <f>COUNTIF(D13:DS13, "C")</f>
@@ -2557,10 +2579,10 @@
       <c r="DP13" s="49"/>
       <c r="DQ13" s="49"/>
       <c r="DR13" s="49"/>
-      <c r="DS13" s="50"/>
+      <c r="DS13" s="42"/>
     </row>
     <row r="14" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="114">
+      <c r="A14" s="109">
         <v>2</v>
       </c>
       <c r="B14" s="22" t="s">
@@ -2728,7 +2750,7 @@
       <c r="DS14" s="40"/>
     </row>
     <row r="15" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="109"/>
+      <c r="A15" s="104"/>
       <c r="B15" s="26"/>
       <c r="C15" s="25">
         <f>COUNTIF(D15:DS15, "C")</f>
@@ -2908,7 +2930,7 @@
       <c r="DS15" s="50"/>
     </row>
     <row r="16" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="107">
+      <c r="A16" s="102">
         <v>3</v>
       </c>
       <c r="B16" s="22" t="s">
@@ -3048,7 +3070,7 @@
       <c r="DS16" s="42"/>
     </row>
     <row r="17" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="109"/>
+      <c r="A17" s="104"/>
       <c r="B17" s="27"/>
       <c r="C17" s="25">
         <f>COUNTIF(D17:DS17, "C")</f>
@@ -3188,7 +3210,7 @@
       <c r="DS17" s="50"/>
     </row>
     <row r="18" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="107">
+      <c r="A18" s="102">
         <v>4</v>
       </c>
       <c r="B18" s="22" t="s">
@@ -3342,7 +3364,7 @@
       <c r="DS18" s="42"/>
     </row>
     <row r="19" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="109"/>
+      <c r="A19" s="104"/>
       <c r="B19" s="27"/>
       <c r="C19" s="25">
         <f>COUNTIF(D19:DS19, "C")</f>
@@ -3502,7 +3524,7 @@
       <c r="DS19" s="50"/>
     </row>
     <row r="20" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="107">
+      <c r="A20" s="102">
         <v>5</v>
       </c>
       <c r="B20" s="22" t="s">
@@ -3656,7 +3678,7 @@
       <c r="DS20" s="42"/>
     </row>
     <row r="21" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="109"/>
+      <c r="A21" s="104"/>
       <c r="B21" s="27"/>
       <c r="C21" s="25">
         <f>COUNTIF(D21:DS21, "C")</f>
@@ -3802,7 +3824,7 @@
       <c r="DS21" s="50"/>
     </row>
     <row r="22" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="107">
+      <c r="A22" s="102">
         <v>6</v>
       </c>
       <c r="B22" s="22" t="s">
@@ -3946,7 +3968,7 @@
       <c r="DS22" s="42"/>
     </row>
     <row r="23" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="109"/>
+      <c r="A23" s="104"/>
       <c r="B23" s="27"/>
       <c r="C23" s="25">
         <f>COUNTIF(D23:DS23, "C")</f>
@@ -4082,7 +4104,7 @@
       <c r="DS23" s="50"/>
     </row>
     <row r="24" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="107">
+      <c r="A24" s="102">
         <v>7</v>
       </c>
       <c r="B24" s="22"/>
@@ -4212,7 +4234,7 @@
       <c r="DS24" s="42"/>
     </row>
     <row r="25" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="109"/>
+      <c r="A25" s="104"/>
       <c r="B25" s="27"/>
       <c r="C25" s="25">
         <f>COUNTIF(D25:DS25, "C")</f>
@@ -4340,7 +4362,7 @@
       <c r="DS25" s="50"/>
     </row>
     <row r="26" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="107">
+      <c r="A26" s="102">
         <v>8</v>
       </c>
       <c r="B26" s="22" t="s">
@@ -4500,11 +4522,11 @@
       <c r="DS26" s="42"/>
     </row>
     <row r="27" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="109"/>
+      <c r="A27" s="104"/>
       <c r="B27" s="27"/>
       <c r="C27" s="25">
         <f>COUNTIF(D27:DS27, "C")</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D27" s="43"/>
       <c r="E27" s="44"/>
@@ -4619,14 +4641,30 @@
       <c r="DD27" s="46"/>
       <c r="DE27" s="46"/>
       <c r="DF27" s="46"/>
-      <c r="DG27" s="46"/>
-      <c r="DH27" s="46"/>
-      <c r="DI27" s="47"/>
-      <c r="DJ27" s="48"/>
-      <c r="DK27" s="45"/>
-      <c r="DL27" s="45"/>
-      <c r="DM27" s="45"/>
-      <c r="DN27" s="46"/>
+      <c r="DG27" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="DH27" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="DI27" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="DJ27" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="DK27" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="DL27" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="DM27" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="DN27" s="46" t="s">
+        <v>14</v>
+      </c>
       <c r="DO27" s="49"/>
       <c r="DP27" s="49"/>
       <c r="DQ27" s="49"/>
@@ -4634,7 +4672,7 @@
       <c r="DS27" s="50"/>
     </row>
     <row r="28" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="107"/>
+      <c r="A28" s="102"/>
       <c r="B28" s="29" t="s">
         <v>5</v>
       </c>
@@ -4764,13 +4802,13 @@
       <c r="DS28" s="42"/>
     </row>
     <row r="29" spans="1:123" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="108"/>
+      <c r="A29" s="103"/>
       <c r="B29" s="30" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="31">
         <f>SUM(C11,C13,C15,C17,C19,C21,C23,C25,C27)</f>
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D29" s="51"/>
       <c r="E29" s="51"/>
@@ -5092,41 +5130,21 @@
     <row r="35" spans="1:63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="CF8:CJ8"/>
-    <mergeCell ref="CK8:CO8"/>
-    <mergeCell ref="CP8:CT8"/>
-    <mergeCell ref="CU8:CY8"/>
-    <mergeCell ref="CF6:CO6"/>
-    <mergeCell ref="CP6:CY6"/>
-    <mergeCell ref="CF7:CO7"/>
-    <mergeCell ref="CP7:CY7"/>
-    <mergeCell ref="BL6:BU6"/>
-    <mergeCell ref="BV6:CE6"/>
-    <mergeCell ref="BL7:BU7"/>
-    <mergeCell ref="BV7:CE7"/>
-    <mergeCell ref="BL8:BP8"/>
-    <mergeCell ref="BQ8:BU8"/>
-    <mergeCell ref="BV8:BZ8"/>
-    <mergeCell ref="CA8:CE8"/>
-    <mergeCell ref="BG8:BK8"/>
-    <mergeCell ref="AR6:BA6"/>
-    <mergeCell ref="BB6:BK6"/>
-    <mergeCell ref="AR7:BA7"/>
-    <mergeCell ref="BB7:BK7"/>
-    <mergeCell ref="AR8:AV8"/>
-    <mergeCell ref="AW8:BA8"/>
-    <mergeCell ref="BB8:BF8"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A6:B8"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="CZ6:DI6"/>
+    <mergeCell ref="DJ6:DS6"/>
+    <mergeCell ref="CZ7:DI7"/>
+    <mergeCell ref="DJ7:DS7"/>
+    <mergeCell ref="CZ8:DD8"/>
+    <mergeCell ref="DE8:DI8"/>
+    <mergeCell ref="DJ8:DN8"/>
+    <mergeCell ref="DO8:DS8"/>
+    <mergeCell ref="BH4:BI4"/>
+    <mergeCell ref="N6:W6"/>
+    <mergeCell ref="N7:W7"/>
+    <mergeCell ref="X6:AG6"/>
+    <mergeCell ref="AH6:AQ6"/>
+    <mergeCell ref="X7:AG7"/>
+    <mergeCell ref="AH7:AQ7"/>
     <mergeCell ref="N8:R8"/>
     <mergeCell ref="S8:W8"/>
     <mergeCell ref="AV2:BC2"/>
@@ -5141,36 +5159,56 @@
     <mergeCell ref="AN2:AT2"/>
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="AV4:BC4"/>
-    <mergeCell ref="BH4:BI4"/>
-    <mergeCell ref="N6:W6"/>
-    <mergeCell ref="N7:W7"/>
-    <mergeCell ref="X6:AG6"/>
-    <mergeCell ref="AH6:AQ6"/>
-    <mergeCell ref="X7:AG7"/>
-    <mergeCell ref="AH7:AQ7"/>
-    <mergeCell ref="CZ6:DI6"/>
-    <mergeCell ref="DJ6:DS6"/>
-    <mergeCell ref="CZ7:DI7"/>
-    <mergeCell ref="DJ7:DS7"/>
-    <mergeCell ref="CZ8:DD8"/>
-    <mergeCell ref="DE8:DI8"/>
-    <mergeCell ref="DJ8:DN8"/>
-    <mergeCell ref="DO8:DS8"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A6:B8"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="BG8:BK8"/>
+    <mergeCell ref="AR6:BA6"/>
+    <mergeCell ref="BB6:BK6"/>
+    <mergeCell ref="AR7:BA7"/>
+    <mergeCell ref="BB7:BK7"/>
+    <mergeCell ref="AR8:AV8"/>
+    <mergeCell ref="AW8:BA8"/>
+    <mergeCell ref="BB8:BF8"/>
+    <mergeCell ref="BL6:BU6"/>
+    <mergeCell ref="BV6:CE6"/>
+    <mergeCell ref="BL7:BU7"/>
+    <mergeCell ref="BV7:CE7"/>
+    <mergeCell ref="BL8:BP8"/>
+    <mergeCell ref="BQ8:BU8"/>
+    <mergeCell ref="BV8:BZ8"/>
+    <mergeCell ref="CA8:CE8"/>
+    <mergeCell ref="CF8:CJ8"/>
+    <mergeCell ref="CK8:CO8"/>
+    <mergeCell ref="CP8:CT8"/>
+    <mergeCell ref="CU8:CY8"/>
+    <mergeCell ref="CF6:CO6"/>
+    <mergeCell ref="CP6:CY6"/>
+    <mergeCell ref="CF7:CO7"/>
+    <mergeCell ref="CP7:CY7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D10:CY29">
-    <cfRule type="containsText" dxfId="3" priority="3" stopIfTrue="1" operator="containsText" text="C">
+    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",D10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" stopIfTrue="1" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",D10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CZ10:DS29">
-    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" operator="containsText" text="C">
+    <cfRule type="containsText" dxfId="3" priority="1" stopIfTrue="1" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",CZ10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" stopIfTrue="1" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="2" priority="2" stopIfTrue="1" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",CZ10)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>